<commit_message>
Update the Client Organization Test Scripts code to include a new functionality & Modified the MPM and MPC test script
</commit_message>
<xml_diff>
--- a/com.absli.auto/src/main/java/com/absli/testdata/Client Organization.xlsx
+++ b/com.absli.auto/src/main/java/com/absli/testdata/Client Organization.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gokulnath\eclipse-workspace\com.absli.auto\src\main\java\com\absli\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gokulnath\git\com.absli.auto\com.absli.auto\src\main\java\com\absli\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TC_CO_001" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="45">
   <si>
     <t>Client Name</t>
   </si>
@@ -104,18 +104,9 @@
     <t>GST</t>
   </si>
   <si>
-    <t>absli-Training-001</t>
-  </si>
-  <si>
     <t>absli-001</t>
   </si>
   <si>
-    <t>ABSLI1324L</t>
-  </si>
-  <si>
-    <t>29ABSLI1324LC1ZU</t>
-  </si>
-  <si>
     <t>132430</t>
   </si>
   <si>
@@ -128,12 +119,6 @@
     <t>2</t>
   </si>
   <si>
-    <t>grade-001</t>
-  </si>
-  <si>
-    <t>GOKUL1324G</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -143,7 +128,40 @@
     <t>NO GST PAYABLE</t>
   </si>
   <si>
-    <t>Absli-011</t>
+    <t>Change Password access required at claim portal</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Absli-Grade-001</t>
+  </si>
+  <si>
+    <t>Absli-GST-Grade-001</t>
+  </si>
+  <si>
+    <t>FGHIJ5678K</t>
+  </si>
+  <si>
+    <t>Absli-Auto-004</t>
+  </si>
+  <si>
+    <t>29FGHIJ5678K1Z4</t>
+  </si>
+  <si>
+    <t>GOKUL1324L</t>
+  </si>
+  <si>
+    <t>KLMNO9101V</t>
+  </si>
+  <si>
+    <t>29KLMNO9101V1Z8</t>
+  </si>
+  <si>
+    <t>GOKUL1324A</t>
+  </si>
+  <si>
+    <t>Absli-Auto-GST-002</t>
   </si>
 </sst>
 </file>
@@ -200,12 +218,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -487,9 +509,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -502,16 +524,17 @@
     <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -534,31 +557,34 @@
         <v>9</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>38</v>
       </c>
@@ -569,39 +595,42 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>15</v>
+      <c r="J2" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="1">
         <v>560076</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -613,15 +642,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection sqref="A1:P2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -629,271 +658,9 @@
     <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" s="1">
-        <v>560076</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" s="1">
-        <v>560076</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22" customWidth="1"/>
+    <col min="9" max="9" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -926,13 +693,13 @@
         <v>22</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>13</v>
@@ -955,7 +722,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -964,7 +731,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>
@@ -972,20 +739,158 @@
       <c r="F2" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="G2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="1">
+        <v>560076</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="G2" s="1" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>15</v>
@@ -1003,6 +908,151 @@
         <v>20</v>
       </c>
       <c r="Q2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="1">
+        <v>560076</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update in GPS and GBY
</commit_message>
<xml_diff>
--- a/com.absli.auto/src/main/java/com/absli/testdata/Client Organization.xlsx
+++ b/com.absli.auto/src/main/java/com/absli/testdata/Client Organization.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575"/>
   </bookViews>
   <sheets>
     <sheet name="TC_CO_001" sheetId="2" r:id="rId1"/>
@@ -134,12 +134,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Absli-Auto-005</t>
-  </si>
-  <si>
-    <t>GOKUL1324R</t>
-  </si>
-  <si>
     <t>Absli-Grade-002</t>
   </si>
   <si>
@@ -162,6 +156,12 @@
   </si>
   <si>
     <t>29GLMNO9101G1Z8</t>
+  </si>
+  <si>
+    <t>GBY-Auto-001</t>
+  </si>
+  <si>
+    <t>GOKUP1324R</t>
   </si>
 </sst>
 </file>
@@ -515,7 +515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -590,7 +590,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -605,7 +605,7 @@
         <v>31</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>32</v>
@@ -648,7 +648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -726,7 +726,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -744,10 +744,10 @@
         <v>24</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>34</v>
@@ -864,7 +864,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -882,7 +882,7 @@
         <v>23</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>34</v>
@@ -1006,7 +1006,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -1024,10 +1024,10 @@
         <v>24</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Updated for folder structure
</commit_message>
<xml_diff>
--- a/com.absli.auto/src/main/java/com/absli/testdata/Client Organization.xlsx
+++ b/com.absli.auto/src/main/java/com/absli/testdata/Client Organization.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TC_CO_001" sheetId="2" r:id="rId1"/>
@@ -134,34 +134,34 @@
     <t>No</t>
   </si>
   <si>
-    <t>Absli-Grade-002</t>
-  </si>
-  <si>
-    <t>GOKUL1324D</t>
-  </si>
-  <si>
-    <t>Absli-GST-Grade-002</t>
-  </si>
-  <si>
-    <t>FGHIJ5678G</t>
-  </si>
-  <si>
-    <t>29FGHIJ5678G1Z4</t>
-  </si>
-  <si>
-    <t>Voluntary Test-001</t>
-  </si>
-  <si>
-    <t>GLMNO9101G</t>
-  </si>
-  <si>
-    <t>29GLMNO9101G1Z8</t>
-  </si>
-  <si>
-    <t>GBY-Auto-001</t>
-  </si>
-  <si>
-    <t>GOKUP1324R</t>
+    <t>Demo-Auto-003</t>
+  </si>
+  <si>
+    <t>Demo-Auto-004</t>
+  </si>
+  <si>
+    <t>Demo-Grade-002</t>
+  </si>
+  <si>
+    <t>Demo-GST-Grade-002</t>
+  </si>
+  <si>
+    <t>CDEFG1234H</t>
+  </si>
+  <si>
+    <t>EFGHI5678I</t>
+  </si>
+  <si>
+    <t>29EFGHI5678I1Z8</t>
+  </si>
+  <si>
+    <t>GHIJK9101J</t>
+  </si>
+  <si>
+    <t>IJKLM2345K</t>
+  </si>
+  <si>
+    <t>29IJKLM2345K1Z4</t>
   </si>
 </sst>
 </file>
@@ -515,7 +515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -590,7 +590,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -604,8 +604,8 @@
       <c r="E2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>44</v>
+      <c r="F2" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>32</v>
@@ -648,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,7 +726,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -744,10 +744,10 @@
         <v>24</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>34</v>
@@ -787,7 +787,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,7 +798,7 @@
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="44.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
@@ -864,7 +864,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -882,7 +882,7 @@
         <v>23</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>34</v>
@@ -925,7 +925,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,7 +936,7 @@
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="44.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
@@ -1006,7 +1006,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -1024,10 +1024,10 @@
         <v>24</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>34</v>

</xml_diff>